<commit_message>
Se completa el archivo de la matriz de riesgo tanto a nivel de proyecto como de producto
</commit_message>
<xml_diff>
--- a/Matriz de Riesgos.xlsx
+++ b/Matriz de Riesgos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training Automatización de pruebas\Semana 5 y 6\Taller final\HomeSentry\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Training Automatización de pruebas\Semana 5 y 6\Taller final\Git\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{03848AE3-67DB-4E75-AA36-52FBABA749BB}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E0A0D17-2DD5-437C-89F1-9238A93254BF}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28635" windowHeight="5235" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Matriz Riesgo" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="133">
   <si>
     <t>Consecutivo</t>
   </si>
@@ -389,6 +389,51 @@
   </si>
   <si>
     <t>La capacidad limitada del sitio web de la tienda para manejar un mayor tráfico o una mayor cantidad de transacciones en el futuro, lo que podría obstaculizar su crecimiento.</t>
+  </si>
+  <si>
+    <t>Crear una estrategia para el crecimiento progresivo de un sitio web, utilizando una arquitectura adaptable que facilite la integración de nuevos recursos y funciones sin perjudicar la eficacia del sitio.</t>
+  </si>
+  <si>
+    <t>Establecer un plan de contingencia para mitigar el alto tráfico en la página web, como la creación de una lista de espera de los usuarios, la restricción del acceso a ciertas funcionalidades no esenciales del sitio y la implementación de un sistema de alerta temprana para detectar posibles problemas de rendimiento.</t>
+  </si>
+  <si>
+    <t>La tienda en línea podría no estar preparada para gestionar un gran flujo de visitantes y compras, lo que podría afectar negativamente la rentabilidad del negocio.</t>
+  </si>
+  <si>
+    <t>Situaciones que afectan la seguridad poniendo en peligro la privacidad de los usuarios o los datos de la tienda en línea.</t>
+  </si>
+  <si>
+    <t>Aplicar medidas de seguridad tales como: encriptación de datos, autenticación de usuarios y realización de auditorías de seguridad periódicas, adicional a esto, establecer políticas claras de seguridad y capacitaciones al personal.</t>
+  </si>
+  <si>
+    <t>Situaciones en las que el servidor no está disponible o no funciona correctamente, lo que puede resultar en una mala experiencia para los usuarios y disminuir las venta.</t>
+  </si>
+  <si>
+    <t>Contar con un plan de contingencia en caso de que se presente una interrupción en el servidor, donde se establezcan un paso a paso de cómo solucionar el problema lo más pronto posible y comunicar de manera efectiva a los usuarios afectados sobre la situación y el tiempo de recuperación estimado.</t>
+  </si>
+  <si>
+    <t>Situaciones en las que la gestión del tráfico y la carga de la página web (tienda en línea) no funcionan adecuadamente, lo que puede generar que cargue lenta la información y una mala experiencia de navegación para los usuarios.</t>
+  </si>
+  <si>
+    <t>Adquirir servidores o servicios de alojamiento que sean capaces de manejar un gran volumen de tráfico y estén diseñados específicamente para garantizar la velocidad de carga y la disponibilidad de la página web.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dificultades para que la página web funcione adecuadamente en distintos idiomas y regiones, lo cual podría reducir la capacidad de la página we (tienda en líena) para llegar a otros usuarios en cualquier lugar del mundo. </t>
+  </si>
+  <si>
+    <t>No es necesario enfocarse mucho en este riesgo ya que es poco probable que ocurra y porque la tienda está enfocada en vender exclusivamente en Colombia, por lo que no es necesario invertir en la adaptación del sitio web a diferentes idiomas y regiones.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Restringir la cantidad de programas desarrollados por personas ajenas que se conectan con la página web, y verificar que solo se usen programas confiables y reconocidos. </t>
+  </si>
+  <si>
+    <t>Encontrar dificultades en la conexión y uso de herramientas externas o de terceros, como PSE, PayPal, Nequi, American Express, entre otros, lo cual podría afectar negativamente la capacidad de la tienda y el proceso de las ventas de manera efectiva.</t>
+  </si>
+  <si>
+    <t>Los problemas con el equipo de soporte técnico pueden tener un impacto negativo en la experiencia de los usuarios y la imagen de la tienda.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Asegurarse de que el equipo de soporte técnico esté compuesto por profesionales capacitados y habilidosos para brindar un buen servicio al cliente y proteger la imagen de la tienda. </t>
   </si>
 </sst>
 </file>
@@ -674,6 +719,12 @@
     </xf>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -682,12 +733,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1415,8 +1460,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:M1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A29" workbookViewId="0">
-      <selection activeCell="I30" sqref="I30"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1435,88 +1480,88 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A1" s="32"/>
-      <c r="B1" s="33"/>
-      <c r="C1" s="33"/>
-      <c r="D1" s="33"/>
-      <c r="E1" s="33"/>
-      <c r="F1" s="33"/>
-      <c r="G1" s="33"/>
-      <c r="H1" s="33"/>
-      <c r="I1" s="33"/>
-      <c r="J1" s="33"/>
-      <c r="K1" s="33"/>
-      <c r="L1" s="33"/>
+      <c r="A1" s="34"/>
+      <c r="B1" s="35"/>
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="35"/>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35"/>
+      <c r="J1" s="35"/>
+      <c r="K1" s="35"/>
+      <c r="L1" s="35"/>
     </row>
     <row r="2" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="33"/>
-      <c r="B2" s="33"/>
-      <c r="C2" s="33"/>
-      <c r="D2" s="33"/>
-      <c r="E2" s="33"/>
-      <c r="F2" s="33"/>
-      <c r="G2" s="33"/>
-      <c r="H2" s="33"/>
-      <c r="I2" s="33"/>
-      <c r="J2" s="33"/>
-      <c r="K2" s="33"/>
-      <c r="L2" s="33"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="35"/>
+      <c r="C2" s="35"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="35"/>
+      <c r="F2" s="35"/>
+      <c r="G2" s="35"/>
+      <c r="H2" s="35"/>
+      <c r="I2" s="35"/>
+      <c r="J2" s="35"/>
+      <c r="K2" s="35"/>
+      <c r="L2" s="35"/>
     </row>
     <row r="3" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="33"/>
-      <c r="B3" s="33"/>
-      <c r="C3" s="33"/>
-      <c r="D3" s="33"/>
-      <c r="E3" s="33"/>
-      <c r="F3" s="33"/>
-      <c r="G3" s="33"/>
-      <c r="H3" s="33"/>
-      <c r="I3" s="33"/>
-      <c r="J3" s="33"/>
-      <c r="K3" s="33"/>
-      <c r="L3" s="33"/>
+      <c r="A3" s="35"/>
+      <c r="B3" s="35"/>
+      <c r="C3" s="35"/>
+      <c r="D3" s="35"/>
+      <c r="E3" s="35"/>
+      <c r="F3" s="35"/>
+      <c r="G3" s="35"/>
+      <c r="H3" s="35"/>
+      <c r="I3" s="35"/>
+      <c r="J3" s="35"/>
+      <c r="K3" s="35"/>
+      <c r="L3" s="35"/>
     </row>
     <row r="4" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="33"/>
-      <c r="B4" s="33"/>
-      <c r="C4" s="33"/>
-      <c r="D4" s="33"/>
-      <c r="E4" s="33"/>
-      <c r="F4" s="33"/>
-      <c r="G4" s="33"/>
-      <c r="H4" s="33"/>
-      <c r="I4" s="33"/>
-      <c r="J4" s="33"/>
-      <c r="K4" s="33"/>
-      <c r="L4" s="33"/>
+      <c r="A4" s="35"/>
+      <c r="B4" s="35"/>
+      <c r="C4" s="35"/>
+      <c r="D4" s="35"/>
+      <c r="E4" s="35"/>
+      <c r="F4" s="35"/>
+      <c r="G4" s="35"/>
+      <c r="H4" s="35"/>
+      <c r="I4" s="35"/>
+      <c r="J4" s="35"/>
+      <c r="K4" s="35"/>
+      <c r="L4" s="35"/>
     </row>
     <row r="5" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="33"/>
-      <c r="B5" s="33"/>
-      <c r="C5" s="33"/>
-      <c r="D5" s="33"/>
-      <c r="E5" s="33"/>
-      <c r="F5" s="33"/>
-      <c r="G5" s="33"/>
-      <c r="H5" s="33"/>
-      <c r="I5" s="33"/>
-      <c r="J5" s="33"/>
-      <c r="K5" s="33"/>
-      <c r="L5" s="33"/>
+      <c r="A5" s="35"/>
+      <c r="B5" s="35"/>
+      <c r="C5" s="35"/>
+      <c r="D5" s="35"/>
+      <c r="E5" s="35"/>
+      <c r="F5" s="35"/>
+      <c r="G5" s="35"/>
+      <c r="H5" s="35"/>
+      <c r="I5" s="35"/>
+      <c r="J5" s="35"/>
+      <c r="K5" s="35"/>
+      <c r="L5" s="35"/>
     </row>
     <row r="6" spans="1:13" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="33"/>
-      <c r="B6" s="33"/>
-      <c r="C6" s="33"/>
-      <c r="D6" s="33"/>
-      <c r="E6" s="33"/>
-      <c r="F6" s="33"/>
-      <c r="G6" s="33"/>
-      <c r="H6" s="33"/>
-      <c r="I6" s="33"/>
-      <c r="J6" s="33"/>
-      <c r="K6" s="33"/>
-      <c r="L6" s="33"/>
+      <c r="A6" s="35"/>
+      <c r="B6" s="35"/>
+      <c r="C6" s="35"/>
+      <c r="D6" s="35"/>
+      <c r="E6" s="35"/>
+      <c r="F6" s="35"/>
+      <c r="G6" s="35"/>
+      <c r="H6" s="35"/>
+      <c r="I6" s="35"/>
+      <c r="J6" s="35"/>
+      <c r="K6" s="35"/>
+      <c r="L6" s="35"/>
     </row>
     <row r="7" spans="1:13" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="20" t="s">
@@ -1560,7 +1605,7 @@
       <c r="A8" s="11">
         <v>1</v>
       </c>
-      <c r="B8" s="36" t="s">
+      <c r="B8" s="32" t="s">
         <v>72</v>
       </c>
       <c r="C8" s="24" t="s">
@@ -1601,7 +1646,7 @@
       <c r="A9" s="1">
         <v>2</v>
       </c>
-      <c r="B9" s="36" t="s">
+      <c r="B9" s="32" t="s">
         <v>67</v>
       </c>
       <c r="C9" s="24" t="s">
@@ -1638,7 +1683,7 @@
       <c r="A10" s="11">
         <v>3</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="32" t="s">
         <v>69</v>
       </c>
       <c r="C10" s="24" t="s">
@@ -1675,7 +1720,7 @@
       <c r="A11" s="11">
         <v>4</v>
       </c>
-      <c r="B11" s="36" t="s">
+      <c r="B11" s="32" t="s">
         <v>76</v>
       </c>
       <c r="C11" s="24" t="s">
@@ -1712,7 +1757,7 @@
       <c r="A12" s="11">
         <v>5</v>
       </c>
-      <c r="B12" s="37" t="s">
+      <c r="B12" s="33" t="s">
         <v>63</v>
       </c>
       <c r="C12" s="24" t="s">
@@ -2398,8 +2443,12 @@
       <c r="H30" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="I30" s="2"/>
-      <c r="J30" s="11"/>
+      <c r="I30" s="2" t="s">
+        <v>118</v>
+      </c>
+      <c r="J30" s="11" t="s">
+        <v>17</v>
+      </c>
       <c r="K30" s="8">
         <v>44990</v>
       </c>
@@ -2407,24 +2456,36 @@
         <v>86</v>
       </c>
     </row>
-    <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A31" s="11">
         <v>24</v>
       </c>
-      <c r="B31" s="9"/>
+      <c r="B31" s="9" t="s">
+        <v>120</v>
+      </c>
       <c r="C31" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
+      <c r="D31" s="11">
+        <v>2</v>
+      </c>
+      <c r="E31" s="11">
+        <v>4</v>
+      </c>
       <c r="F31" s="3"/>
       <c r="G31" s="3">
         <f>'Matriz Riesgo'!$D31*'Matriz Riesgo'!$E31</f>
-        <v>0</v>
-      </c>
-      <c r="H31" s="11"/>
-      <c r="I31" s="2"/>
-      <c r="J31" s="11"/>
+        <v>8</v>
+      </c>
+      <c r="H31" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="I31" s="2" t="s">
+        <v>119</v>
+      </c>
+      <c r="J31" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="K31" s="8">
         <v>44990</v>
       </c>
@@ -2432,24 +2493,36 @@
         <v>86</v>
       </c>
     </row>
-    <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A32" s="11">
         <v>25</v>
       </c>
-      <c r="B32" s="9"/>
+      <c r="B32" s="9" t="s">
+        <v>121</v>
+      </c>
       <c r="C32" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="D32" s="11"/>
-      <c r="E32" s="11"/>
+      <c r="D32" s="11">
+        <v>3</v>
+      </c>
+      <c r="E32" s="11">
+        <v>5</v>
+      </c>
       <c r="F32" s="3"/>
       <c r="G32" s="3">
         <f>'Matriz Riesgo'!$D32*'Matriz Riesgo'!$E32</f>
-        <v>0</v>
-      </c>
-      <c r="H32" s="11"/>
-      <c r="I32" s="2"/>
-      <c r="J32" s="11"/>
+        <v>15</v>
+      </c>
+      <c r="H32" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I32" s="2" t="s">
+        <v>122</v>
+      </c>
+      <c r="J32" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="K32" s="8">
         <v>44990</v>
       </c>
@@ -2457,24 +2530,36 @@
         <v>86</v>
       </c>
     </row>
-    <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A33" s="11">
         <v>26</v>
       </c>
-      <c r="B33" s="9"/>
+      <c r="B33" s="9" t="s">
+        <v>123</v>
+      </c>
       <c r="C33" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
+      <c r="D33" s="11">
+        <v>3</v>
+      </c>
+      <c r="E33" s="11">
+        <v>4</v>
+      </c>
       <c r="F33" s="3"/>
       <c r="G33" s="3">
         <f>'Matriz Riesgo'!$D33*'Matriz Riesgo'!$E33</f>
-        <v>0</v>
-      </c>
-      <c r="H33" s="11"/>
-      <c r="I33" s="2"/>
-      <c r="J33" s="11"/>
+        <v>12</v>
+      </c>
+      <c r="H33" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="I33" s="2" t="s">
+        <v>124</v>
+      </c>
+      <c r="J33" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="K33" s="8">
         <v>44990</v>
       </c>
@@ -2482,24 +2567,36 @@
         <v>86</v>
       </c>
     </row>
-    <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A34" s="11">
         <v>27</v>
       </c>
-      <c r="B34" s="9"/>
+      <c r="B34" s="9" t="s">
+        <v>125</v>
+      </c>
       <c r="C34" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="D34" s="11"/>
-      <c r="E34" s="11"/>
+      <c r="D34" s="11">
+        <v>2</v>
+      </c>
+      <c r="E34" s="11">
+        <v>5</v>
+      </c>
       <c r="F34" s="3"/>
       <c r="G34" s="3">
         <f>'Matriz Riesgo'!$D34*'Matriz Riesgo'!$E34</f>
-        <v>0</v>
-      </c>
-      <c r="H34" s="11"/>
-      <c r="I34" s="2"/>
-      <c r="J34" s="11"/>
+        <v>10</v>
+      </c>
+      <c r="H34" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>126</v>
+      </c>
+      <c r="J34" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="K34" s="8">
         <v>44990</v>
       </c>
@@ -2507,24 +2604,36 @@
         <v>86</v>
       </c>
     </row>
-    <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:12" ht="60" x14ac:dyDescent="0.25">
       <c r="A35" s="11">
         <v>28</v>
       </c>
-      <c r="B35" s="9"/>
+      <c r="B35" s="9" t="s">
+        <v>127</v>
+      </c>
       <c r="C35" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="D35" s="11"/>
-      <c r="E35" s="11"/>
+      <c r="D35" s="11">
+        <v>1</v>
+      </c>
+      <c r="E35" s="11">
+        <v>2</v>
+      </c>
       <c r="F35" s="3"/>
       <c r="G35" s="3">
         <f>'Matriz Riesgo'!$D35*'Matriz Riesgo'!$E35</f>
-        <v>0</v>
-      </c>
-      <c r="H35" s="11"/>
-      <c r="I35" s="2"/>
-      <c r="J35" s="11"/>
+        <v>2</v>
+      </c>
+      <c r="H35" s="11" t="s">
+        <v>43</v>
+      </c>
+      <c r="I35" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="J35" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="K35" s="8">
         <v>44990</v>
       </c>
@@ -2532,24 +2641,36 @@
         <v>86</v>
       </c>
     </row>
-    <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" ht="77.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11">
         <v>29</v>
       </c>
-      <c r="B36" s="9"/>
+      <c r="B36" s="9" t="s">
+        <v>130</v>
+      </c>
       <c r="C36" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="D36" s="11"/>
-      <c r="E36" s="11"/>
+      <c r="D36" s="11">
+        <v>3</v>
+      </c>
+      <c r="E36" s="11">
+        <v>5</v>
+      </c>
       <c r="F36" s="3"/>
       <c r="G36" s="3">
         <f>'Matriz Riesgo'!$D36*'Matriz Riesgo'!$E36</f>
-        <v>0</v>
-      </c>
-      <c r="H36" s="11"/>
-      <c r="I36" s="2"/>
-      <c r="J36" s="11"/>
+        <v>15</v>
+      </c>
+      <c r="H36" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="J36" s="11" t="s">
+        <v>110</v>
+      </c>
       <c r="K36" s="8">
         <v>44990</v>
       </c>
@@ -2557,21 +2678,36 @@
         <v>86</v>
       </c>
     </row>
-    <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:12" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="11">
         <v>30</v>
       </c>
-      <c r="B37" s="9"/>
+      <c r="B37" s="9" t="s">
+        <v>131</v>
+      </c>
       <c r="C37" s="24" t="s">
         <v>87</v>
       </c>
-      <c r="D37" s="11"/>
-      <c r="E37" s="11"/>
+      <c r="D37" s="11">
+        <v>1</v>
+      </c>
+      <c r="E37" s="11">
+        <v>3</v>
+      </c>
       <c r="F37" s="3"/>
-      <c r="G37" s="3"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="2"/>
-      <c r="J37" s="11"/>
+      <c r="G37" s="3">
+        <f>'Matriz Riesgo'!$D37*'Matriz Riesgo'!$E37</f>
+        <v>3</v>
+      </c>
+      <c r="H37" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="J37" s="11" t="s">
+        <v>66</v>
+      </c>
       <c r="K37" s="8">
         <v>44990</v>
       </c>
@@ -7894,10 +8030,10 @@
       <c r="A14" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="F14" s="34" t="s">
+      <c r="F14" s="36" t="s">
         <v>23</v>
       </c>
-      <c r="G14" s="35"/>
+      <c r="G14" s="37"/>
     </row>
     <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="F15" s="13" t="s">

</xml_diff>